<commit_message>
updated the parts list for the smarticle adding resistors and capacitors and transistor
</commit_message>
<xml_diff>
--- a/arduinoSmarticle/parts list.xlsx
+++ b/arduinoSmarticle/parts list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -105,6 +105,54 @@
   </si>
   <si>
     <t>WM7620CT-ND</t>
+  </si>
+  <si>
+    <t>PN2222AD26ZCT-ND</t>
+  </si>
+  <si>
+    <t>PN2222ATFR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npn transistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHM1DCT-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ohm 0603 </t>
+  </si>
+  <si>
+    <t>ESR03EZPJ1R0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHM10KDCT-ND </t>
+  </si>
+  <si>
+    <t>10kohm 0603</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ103</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 35V X5R 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-9064-1-ND </t>
+  </si>
+  <si>
+    <t>C1608X5R1V475K080AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692 </t>
   </si>
 </sst>
 </file>
@@ -441,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +542,7 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -559,14 +607,86 @@
       </c>
       <c r="D9" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" display="https://www.sparkfun.com/products/9868"/>
     <hyperlink ref="A4" r:id="rId2" display="https://www.sparkfun.com/products/11114"/>
+    <hyperlink ref="B10" r:id="rId3" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004"/>
+    <hyperlink ref="A10" r:id="rId4" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
+    <hyperlink ref="C12" r:id="rId6" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
+    <hyperlink ref="B12" r:id="rId7" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
+    <hyperlink ref="A11" r:id="rId8" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
+    <hyperlink ref="C11" r:id="rId9" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
+    <hyperlink ref="A13" r:id="rId11" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
+    <hyperlink ref="C13" r:id="rId12" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
+    <hyperlink ref="B13" r:id="rId13" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
+    <hyperlink ref="D12" r:id="rId14"/>
+    <hyperlink ref="D11" r:id="rId15"/>
+    <hyperlink ref="D10" r:id="rId16"/>
+    <hyperlink ref="D13" r:id="rId17"/>
+    <hyperlink ref="D3" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
smarticle's parts list now include vibration motor
</commit_message>
<xml_diff>
--- a/arduinoSmarticle/parts list.xlsx
+++ b/arduinoSmarticle/parts list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692 </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00Z5AVTY6/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uxcell DC 3V 1500RPM Micro Cell Phone Coreless Vibration Motor 6mmx12mm 5 Pcs </t>
+  </si>
+  <si>
+    <t>TRTV3283</t>
   </si>
 </sst>
 </file>
@@ -489,15 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="155.42578125" bestFit="1" customWidth="1"/>
@@ -663,6 +672,17 @@
       </c>
       <c r="D13" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -685,8 +705,9 @@
     <hyperlink ref="D10" r:id="rId16"/>
     <hyperlink ref="D13" r:id="rId17"/>
     <hyperlink ref="D3" r:id="rId18"/>
+    <hyperlink ref="D14" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated parts list and new version of smarticle with speaker and led
</commit_message>
<xml_diff>
--- a/arduinoSmarticle/parts list.xlsx
+++ b/arduinoSmarticle/parts list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\arduinoSmart\arduinoSmarticle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max Seidel\Documents\Georgia Tech\Smarticles\ArduinoSmarticle\arduinoSmarticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E541CCC4-3DD5-4A2F-91BA-711DF4072D33}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
@@ -162,13 +163,37 @@
   </si>
   <si>
     <t>TRTV3283</t>
+  </si>
+  <si>
+    <t>CC-0601</t>
+  </si>
+  <si>
+    <t>490-CC-0601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3kHz Buzzer </t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/CUI/CC-0601?qs=WyjlAZoYn53PaRhQg76zdw%3D%3D</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>1416-1222-1-ND</t>
+  </si>
+  <si>
+    <t>L130-6580001400001</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lumileds/L130-6580001400001/1416-1222-1-ND/4754534</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +216,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -200,7 +246,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -208,15 +254,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -497,23 +561,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="78.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="155.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="154.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="155.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="154.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -541,7 +605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -555,7 +619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -566,7 +630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -574,7 +638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -582,7 +646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -590,7 +654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -604,7 +668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -618,7 +682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -632,7 +696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -646,7 +710,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -660,7 +724,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -674,7 +738,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -685,27 +749,55 @@
         <v>43</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="https://www.sparkfun.com/products/9868"/>
-    <hyperlink ref="A4" r:id="rId2" display="https://www.sparkfun.com/products/11114"/>
-    <hyperlink ref="B10" r:id="rId3" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004"/>
-    <hyperlink ref="A10" r:id="rId4" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004"/>
-    <hyperlink ref="A12" r:id="rId5" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
-    <hyperlink ref="C12" r:id="rId6" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
-    <hyperlink ref="B12" r:id="rId7" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
-    <hyperlink ref="A11" r:id="rId8" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
-    <hyperlink ref="C11" r:id="rId9" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
-    <hyperlink ref="A13" r:id="rId11" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
-    <hyperlink ref="C13" r:id="rId12" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
-    <hyperlink ref="B13" r:id="rId13" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
-    <hyperlink ref="D12" r:id="rId14"/>
-    <hyperlink ref="D11" r:id="rId15"/>
-    <hyperlink ref="D10" r:id="rId16"/>
-    <hyperlink ref="D13" r:id="rId17"/>
-    <hyperlink ref="D3" r:id="rId18"/>
-    <hyperlink ref="D14" r:id="rId19"/>
+    <hyperlink ref="A5" r:id="rId1" display="https://www.sparkfun.com/products/9868" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId2" display="https://www.sparkfun.com/products/11114" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId3" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A10" r:id="rId4" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C12" r:id="rId6" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A11" r:id="rId8" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C11" r:id="rId9" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A13" r:id="rId11" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B13" r:id="rId13" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D12" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D3" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>

</xml_diff>

<commit_message>
added jst connector to the parts list
</commit_message>
<xml_diff>
--- a/arduinoSmarticle/parts list.xlsx
+++ b/arduinoSmarticle/parts list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max Seidel\Documents\Georgia Tech\Smarticles\ArduinoSmarticle\arduinoSmarticle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\arduinoSmart\arduinoSmarticle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E541CCC4-3DD5-4A2F-91BA-711DF4072D33}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>name</t>
   </si>
@@ -187,12 +186,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/lumileds/L130-6580001400001/1416-1222-1-ND/4754534</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/eBoot-Pairs-Electrical-Female-Connector/dp/B06WGM9W7S/ref=sr_1_1?ie=UTF8&amp;qid=1531752427&amp;sr=8-1&amp;keywords=20+pair+micro+jst+1.25</t>
+  </si>
+  <si>
+    <t>jst 2 pin 1.25mm electrical female plug</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -561,23 +566,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="78.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="155.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="154.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="155.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="154.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -605,7 +610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -619,7 +624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -630,7 +635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -638,7 +643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -646,7 +651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -654,7 +659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -668,7 +673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -682,7 +687,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -696,7 +701,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -710,7 +715,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -724,7 +729,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -738,7 +743,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -749,7 +754,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -763,7 +768,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -777,27 +782,35 @@
         <v>53</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="https://www.sparkfun.com/products/9868" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A4" r:id="rId2" display="https://www.sparkfun.com/products/11114" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B10" r:id="rId3" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A10" r:id="rId4" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A12" r:id="rId5" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C12" r:id="rId6" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B12" r:id="rId7" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A11" r:id="rId8" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C11" r:id="rId9" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A13" r:id="rId11" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId12" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B13" r:id="rId13" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D12" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D3" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A5" r:id="rId1" display="https://www.sparkfun.com/products/9868"/>
+    <hyperlink ref="A4" r:id="rId2" display="https://www.sparkfun.com/products/11114"/>
+    <hyperlink ref="B10" r:id="rId3" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004"/>
+    <hyperlink ref="A10" r:id="rId4" display="https://www.digikey.com/product-detail/en/on-semiconductor/PN2222ATFR/PN2222AD26ZCT-ND/459004"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
+    <hyperlink ref="C12" r:id="rId6" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
+    <hyperlink ref="B12" r:id="rId7" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ1R0/RHM1DCT-ND/4053738"/>
+    <hyperlink ref="A11" r:id="rId8" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
+    <hyperlink ref="C11" r:id="rId9" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPJ103/RHM10KDCT-ND/1762925"/>
+    <hyperlink ref="A13" r:id="rId11" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
+    <hyperlink ref="C13" r:id="rId12" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
+    <hyperlink ref="B13" r:id="rId13" display="https://www.digikey.com/product-detail/en/tdk-corporation/C1608X5R1V475K080AC/445-9064-1-ND/3648692"/>
+    <hyperlink ref="D12" r:id="rId14"/>
+    <hyperlink ref="D11" r:id="rId15"/>
+    <hyperlink ref="D10" r:id="rId16"/>
+    <hyperlink ref="D13" r:id="rId17"/>
+    <hyperlink ref="D3" r:id="rId18"/>
+    <hyperlink ref="D14" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>

</xml_diff>